<commit_message>
debug env, TS, LAPH, LFOH, remove exact
</commit_message>
<xml_diff>
--- a/DATA/DataMaster.xlsx
+++ b/DATA/DataMaster.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr hidePivotFieldList="1"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D\University\4th year\Thesis\Hopefully\Thesis\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CEEADB-2F2E-436D-AA69-BDB9F194B26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38594C45-A2FC-49B7-A563-F84636284F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MachineMaster" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="212">
   <si>
     <t>MachineID</t>
   </si>
@@ -674,9 +674,6 @@
   </si>
   <si>
     <t>TotalOperation</t>
-  </si>
-  <si>
-    <t>y</t>
   </si>
 </sst>
 </file>
@@ -3239,10 +3236,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1E3C2B-EB2A-4B5B-9A38-8DCE83FFCF73}">
-  <dimension ref="A1:H169"/>
+  <dimension ref="A1:G169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="E170" sqref="E170"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3338,7 +3335,7 @@
         <v>565</v>
       </c>
       <c r="E4" s="199">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="F4" s="199">
         <v>6</v>
@@ -3414,7 +3411,7 @@
         <v>350</v>
       </c>
       <c r="E7" s="202">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="F7" s="202">
         <f>_xlfn.XLOOKUP(B7,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -3422,7 +3419,7 @@
       </c>
       <c r="G7" s="202">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -3440,7 +3437,7 @@
         <v>350</v>
       </c>
       <c r="E8" s="202">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="F8" s="202">
         <f>_xlfn.XLOOKUP(B8,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -3448,7 +3445,7 @@
       </c>
       <c r="G8" s="202">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -3518,7 +3515,7 @@
         <v>755</v>
       </c>
       <c r="E11" s="199">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="F11" s="199">
         <f>_xlfn.XLOOKUP(B11,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -3526,7 +3523,7 @@
       </c>
       <c r="G11" s="199">
         <f t="shared" si="0"/>
-        <v>1855</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -3596,7 +3593,7 @@
         <v>155</v>
       </c>
       <c r="E14" s="202">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="F14" s="202">
         <f>_xlfn.XLOOKUP(B14,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -3604,7 +3601,7 @@
       </c>
       <c r="G14" s="202">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -3674,7 +3671,7 @@
         <v>565</v>
       </c>
       <c r="E17" s="199">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="F17" s="199">
         <f>_xlfn.XLOOKUP(B17,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -3682,7 +3679,7 @@
       </c>
       <c r="G17" s="199">
         <f t="shared" si="0"/>
-        <v>1440</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -3752,7 +3749,7 @@
         <v>330</v>
       </c>
       <c r="E20" s="202">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="F20" s="202">
         <f>_xlfn.XLOOKUP(B20,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -3760,7 +3757,7 @@
       </c>
       <c r="G20" s="202">
         <f t="shared" si="0"/>
-        <v>2170</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -3856,7 +3853,7 @@
         <v>350</v>
       </c>
       <c r="E24" s="199">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="F24" s="199">
         <f>_xlfn.XLOOKUP(B24,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -3864,7 +3861,7 @@
       </c>
       <c r="G24" s="199">
         <f t="shared" si="0"/>
-        <v>1140</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -3960,7 +3957,7 @@
         <v>755</v>
       </c>
       <c r="E28" s="202">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="F28" s="202">
         <f>_xlfn.XLOOKUP(B28,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -3968,7 +3965,7 @@
       </c>
       <c r="G28" s="202">
         <f t="shared" si="0"/>
-        <v>1750</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -3986,7 +3983,7 @@
         <v>80</v>
       </c>
       <c r="E29" s="199">
-        <v>710</v>
+        <v>800</v>
       </c>
       <c r="F29" s="199">
         <f>_xlfn.XLOOKUP(B29,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -3994,7 +3991,7 @@
       </c>
       <c r="G29" s="199">
         <f t="shared" si="0"/>
-        <v>1420</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -4064,7 +4061,7 @@
         <v>330</v>
       </c>
       <c r="E32" s="202">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F32" s="202">
         <f>_xlfn.XLOOKUP(B32,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4072,7 +4069,7 @@
       </c>
       <c r="G32" s="202">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4090,7 +4087,7 @@
         <v>565</v>
       </c>
       <c r="E33" s="202">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="F33" s="202">
         <f>_xlfn.XLOOKUP(B33,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4098,7 +4095,7 @@
       </c>
       <c r="G33" s="202">
         <f t="shared" si="0"/>
-        <v>1440</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4168,7 +4165,7 @@
         <v>150</v>
       </c>
       <c r="E36" s="199">
-        <v>500</v>
+        <v>510</v>
       </c>
       <c r="F36" s="199">
         <f>_xlfn.XLOOKUP(B36,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4176,7 +4173,7 @@
       </c>
       <c r="G36" s="199">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4271,7 +4268,7 @@
         <v>495</v>
       </c>
       <c r="E40" s="202">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="F40" s="202">
         <f>_xlfn.XLOOKUP(B40,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4279,7 +4276,7 @@
       </c>
       <c r="G40" s="202">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4323,7 +4320,7 @@
         <v>495</v>
       </c>
       <c r="E42" s="200">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="F42" s="200">
         <f>_xlfn.XLOOKUP(B42,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4331,7 +4328,7 @@
       </c>
       <c r="G42" s="200">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4401,7 +4398,7 @@
         <v>565</v>
       </c>
       <c r="E45" s="202">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="F45" s="202">
         <f>_xlfn.XLOOKUP(B45,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4409,7 +4406,7 @@
       </c>
       <c r="G45" s="202">
         <f t="shared" si="0"/>
-        <v>840</v>
+        <v>900</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4479,7 +4476,7 @@
         <v>755</v>
       </c>
       <c r="E48" s="199">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="F48" s="199">
         <f>_xlfn.XLOOKUP(B48,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4487,7 +4484,7 @@
       </c>
       <c r="G48" s="199">
         <f t="shared" si="0"/>
-        <v>1750</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -4505,7 +4502,7 @@
         <v>565</v>
       </c>
       <c r="E49" s="202">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F49" s="202">
         <f>_xlfn.XLOOKUP(B49,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4513,7 +4510,7 @@
       </c>
       <c r="G49" s="202">
         <f t="shared" si="0"/>
-        <v>1320</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -4658,7 +4655,7 @@
         <v>565</v>
       </c>
       <c r="E55" s="199">
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="F55" s="199">
         <f>_xlfn.XLOOKUP(B55,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4666,7 +4663,7 @@
       </c>
       <c r="G55" s="199">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -4736,7 +4733,7 @@
         <v>755</v>
       </c>
       <c r="E58" s="202">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="F58" s="202">
         <f>_xlfn.XLOOKUP(B58,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4744,7 +4741,7 @@
       </c>
       <c r="G58" s="202">
         <f t="shared" si="0"/>
-        <v>1610</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -4762,7 +4759,7 @@
         <v>150</v>
       </c>
       <c r="E59" s="199">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="F59" s="199">
         <f>_xlfn.XLOOKUP(B59,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4770,7 +4767,7 @@
       </c>
       <c r="G59" s="199">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -4840,7 +4837,7 @@
         <v>155</v>
       </c>
       <c r="E62" s="199">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="F62" s="199">
         <f>_xlfn.XLOOKUP(B62,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4848,7 +4845,7 @@
       </c>
       <c r="G62" s="199">
         <f t="shared" si="0"/>
-        <v>1140</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -4892,7 +4889,7 @@
         <v>20</v>
       </c>
       <c r="E64" s="202">
-        <v>490</v>
+        <v>500</v>
       </c>
       <c r="F64" s="202">
         <f>_xlfn.XLOOKUP(B64,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4900,7 +4897,7 @@
       </c>
       <c r="G64" s="202">
         <f t="shared" si="0"/>
-        <v>490</v>
+        <v>500</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -4917,7 +4914,7 @@
         <v>30</v>
       </c>
       <c r="E65" s="202">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="F65" s="202">
         <f>_xlfn.XLOOKUP(B65,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4925,7 +4922,7 @@
       </c>
       <c r="G65" s="202">
         <f t="shared" ref="G65" si="1">E65*F65</f>
-        <v>560</v>
+        <v>580</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -4942,7 +4939,7 @@
         <v>565</v>
       </c>
       <c r="E66" s="202">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="F66" s="202">
         <f>_xlfn.XLOOKUP(B66,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4950,7 +4947,7 @@
       </c>
       <c r="G66" s="202">
         <f t="shared" ref="G66" si="2">E66*F66</f>
-        <v>1590</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -4967,7 +4964,7 @@
         <v>330</v>
       </c>
       <c r="E67" s="199">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="F67" s="199">
         <f>_xlfn.XLOOKUP(B67,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -4975,7 +4972,7 @@
       </c>
       <c r="G67" s="199">
         <f t="shared" si="0"/>
-        <v>2100</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -5042,7 +5039,7 @@
         <v>145</v>
       </c>
       <c r="E70" s="199">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="F70" s="199">
         <f>_xlfn.XLOOKUP(B70,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5050,7 +5047,7 @@
       </c>
       <c r="G70" s="199">
         <f t="shared" si="3"/>
-        <v>510</v>
+        <v>525</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -5167,7 +5164,7 @@
         <v>755</v>
       </c>
       <c r="E75" s="202">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="F75" s="202">
         <f>_xlfn.XLOOKUP(B75,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5175,7 +5172,7 @@
       </c>
       <c r="G75" s="202">
         <f t="shared" si="3"/>
-        <v>1400</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -5192,7 +5189,7 @@
         <v>350</v>
       </c>
       <c r="E76" s="199">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="F76" s="199">
         <f>_xlfn.XLOOKUP(B76,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5200,7 +5197,7 @@
       </c>
       <c r="G76" s="199">
         <f t="shared" si="3"/>
-        <v>1260</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -5242,7 +5239,7 @@
         <v>155</v>
       </c>
       <c r="E78" s="199">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="F78" s="199">
         <f>_xlfn.XLOOKUP(B78,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5250,7 +5247,7 @@
       </c>
       <c r="G78" s="199">
         <f t="shared" si="3"/>
-        <v>540</v>
+        <v>600</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -5342,7 +5339,7 @@
         <v>150</v>
       </c>
       <c r="E82" s="202">
-        <v>618</v>
+        <v>625</v>
       </c>
       <c r="F82" s="202">
         <f>_xlfn.XLOOKUP(B82,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5350,7 +5347,7 @@
       </c>
       <c r="G82" s="202">
         <f t="shared" ref="G82:G83" si="4">E82*F82</f>
-        <v>1854</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -5367,7 +5364,7 @@
         <v>145</v>
       </c>
       <c r="E83" s="202">
-        <v>516</v>
+        <v>525</v>
       </c>
       <c r="F83" s="202">
         <f>_xlfn.XLOOKUP(B83,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5375,7 +5372,7 @@
       </c>
       <c r="G83" s="202">
         <f t="shared" si="4"/>
-        <v>1548</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -5444,7 +5441,7 @@
         <v>565</v>
       </c>
       <c r="E86" s="199">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="F86" s="199">
         <f>_xlfn.XLOOKUP(B86,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5452,7 +5449,7 @@
       </c>
       <c r="G86" s="199">
         <f t="shared" si="3"/>
-        <v>1206</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -5470,7 +5467,7 @@
         <v>330</v>
       </c>
       <c r="E87" s="199">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="F87" s="199">
         <f>_xlfn.XLOOKUP(B87,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5478,7 +5475,7 @@
       </c>
       <c r="G87" s="199">
         <f t="shared" ref="G87:G88" si="5">E87*F87</f>
-        <v>245</v>
+        <v>294</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -5521,7 +5518,7 @@
         <v>755</v>
       </c>
       <c r="E89" s="202">
-        <v>180</v>
+        <v>110</v>
       </c>
       <c r="F89" s="202">
         <f>_xlfn.XLOOKUP(B89,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5529,7 +5526,7 @@
       </c>
       <c r="G89" s="202">
         <f t="shared" si="3"/>
-        <v>1260</v>
+        <v>770</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -5547,7 +5544,7 @@
         <v>330</v>
       </c>
       <c r="E90" s="202">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F90" s="202">
         <f>_xlfn.XLOOKUP(B90,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5555,7 +5552,7 @@
       </c>
       <c r="G90" s="202">
         <f t="shared" si="3"/>
-        <v>672</v>
+        <v>700</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -5623,7 +5620,7 @@
         <v>565</v>
       </c>
       <c r="E93" s="199">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="F93" s="199">
         <f>_xlfn.XLOOKUP(B93,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5631,7 +5628,7 @@
       </c>
       <c r="G93" s="199">
         <f t="shared" si="3"/>
-        <v>1050</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -5648,7 +5645,7 @@
         <v>350</v>
       </c>
       <c r="E94" s="199">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F94" s="199">
         <f>_xlfn.XLOOKUP(B94,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5656,7 +5653,7 @@
       </c>
       <c r="G94" s="199">
         <f t="shared" si="3"/>
-        <v>408</v>
+        <v>432</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -5698,7 +5695,7 @@
         <v>30</v>
       </c>
       <c r="E96" s="202">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="F96" s="202">
         <f>_xlfn.XLOOKUP(B96,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5706,7 +5703,7 @@
       </c>
       <c r="G96" s="202">
         <f t="shared" si="3"/>
-        <v>448</v>
+        <v>474</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -5723,7 +5720,7 @@
         <v>565</v>
       </c>
       <c r="E97" s="202">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="F97" s="202">
         <f>_xlfn.XLOOKUP(B97,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5731,7 +5728,7 @@
       </c>
       <c r="G97" s="202">
         <f t="shared" si="3"/>
-        <v>1380</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -5798,7 +5795,7 @@
         <v>330</v>
       </c>
       <c r="E100" s="199">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="F100" s="199">
         <f>_xlfn.XLOOKUP(B100,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5806,7 +5803,7 @@
       </c>
       <c r="G100" s="199">
         <f t="shared" si="7"/>
-        <v>2044</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -5850,7 +5847,7 @@
         <v>145</v>
       </c>
       <c r="E102" s="199">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="F102" s="199">
         <f>_xlfn.XLOOKUP(B102,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5858,7 +5855,7 @@
       </c>
       <c r="G102" s="199">
         <f t="shared" si="3"/>
-        <v>1548</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -5928,7 +5925,7 @@
         <v>330</v>
       </c>
       <c r="E105" s="202">
-        <v>300</v>
+        <v>345</v>
       </c>
       <c r="F105" s="202">
         <f>_xlfn.XLOOKUP(B105,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -5936,7 +5933,7 @@
       </c>
       <c r="G105" s="202">
         <f t="shared" si="3"/>
-        <v>2100</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
@@ -6004,7 +6001,7 @@
         <v>350</v>
       </c>
       <c r="E108" s="199">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="F108" s="199">
         <f>_xlfn.XLOOKUP(B108,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6012,7 +6009,7 @@
       </c>
       <c r="G108" s="199">
         <f t="shared" si="3"/>
-        <v>1110</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
@@ -6158,7 +6155,7 @@
         <v>330</v>
       </c>
       <c r="E114" s="202">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="F114" s="202">
         <f>_xlfn.XLOOKUP(B114,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6166,7 +6163,7 @@
       </c>
       <c r="G114" s="202">
         <f t="shared" si="3"/>
-        <v>1610</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
@@ -6209,7 +6206,7 @@
         <v>755</v>
       </c>
       <c r="E116" s="199">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="F116" s="199">
         <f>_xlfn.XLOOKUP(B116,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6217,7 +6214,7 @@
       </c>
       <c r="G116" s="199">
         <f t="shared" si="3"/>
-        <v>735</v>
+        <v>805</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
@@ -6259,7 +6256,7 @@
         <v>155</v>
       </c>
       <c r="E118" s="202">
-        <v>700</v>
+        <v>730</v>
       </c>
       <c r="F118" s="202">
         <f>_xlfn.XLOOKUP(B118,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6267,7 +6264,7 @@
       </c>
       <c r="G118" s="202">
         <f t="shared" si="3"/>
-        <v>2100</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
@@ -6384,7 +6381,7 @@
         <v>350</v>
       </c>
       <c r="E123" s="199">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="F123" s="199">
         <f>_xlfn.XLOOKUP(B123,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6392,7 +6389,7 @@
       </c>
       <c r="G123" s="199">
         <f t="shared" si="3"/>
-        <v>900</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
@@ -6509,7 +6506,7 @@
         <v>350</v>
       </c>
       <c r="E128" s="202">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F128" s="202">
         <f>_xlfn.XLOOKUP(B128,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6517,7 +6514,7 @@
       </c>
       <c r="G128" s="202">
         <f t="shared" si="3"/>
-        <v>1260</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -6584,7 +6581,7 @@
         <v>20</v>
       </c>
       <c r="E131" s="199">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="F131" s="199">
         <f>_xlfn.XLOOKUP(B131,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6592,7 +6589,7 @@
       </c>
       <c r="G131" s="199">
         <f t="shared" si="3"/>
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
@@ -6609,7 +6606,7 @@
         <v>495</v>
       </c>
       <c r="E132" s="199">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="F132" s="199">
         <f>_xlfn.XLOOKUP(B132,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6617,7 +6614,7 @@
       </c>
       <c r="G132" s="199">
         <f t="shared" si="3"/>
-        <v>1500</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
@@ -6634,7 +6631,7 @@
         <v>565</v>
       </c>
       <c r="E133" s="202">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="F133" s="202">
         <f>_xlfn.XLOOKUP(B133,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6642,7 +6639,7 @@
       </c>
       <c r="G133" s="202">
         <f t="shared" si="3"/>
-        <v>720</v>
+        <v>780</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
@@ -6709,7 +6706,7 @@
         <v>350</v>
       </c>
       <c r="E136" s="199">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="F136" s="199">
         <f>_xlfn.XLOOKUP(B136,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6717,7 +6714,7 @@
       </c>
       <c r="G136" s="199">
         <f t="shared" si="3"/>
-        <v>1200</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
@@ -6784,7 +6781,7 @@
         <v>155</v>
       </c>
       <c r="E139" s="202">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F139" s="202">
         <f>_xlfn.XLOOKUP(B139,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6792,7 +6789,7 @@
       </c>
       <c r="G139" s="202">
         <f t="shared" si="3"/>
-        <v>750</v>
+        <v>768</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
@@ -6834,7 +6831,7 @@
         <v>755</v>
       </c>
       <c r="E141" s="202">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="F141" s="202">
         <f>_xlfn.XLOOKUP(B141,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6842,7 +6839,7 @@
       </c>
       <c r="G141" s="202">
         <f t="shared" ref="G141:G168" si="9">E141*F141</f>
-        <v>1400</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
@@ -6859,7 +6856,7 @@
         <v>755</v>
       </c>
       <c r="E142" s="199">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="F142" s="199">
         <f>_xlfn.XLOOKUP(B142,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6867,7 +6864,7 @@
       </c>
       <c r="G142" s="199">
         <f t="shared" si="9"/>
-        <v>875</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
@@ -6934,7 +6931,7 @@
         <v>565</v>
       </c>
       <c r="E145" s="202">
-        <v>210</v>
+        <v>236</v>
       </c>
       <c r="F145" s="202">
         <f>_xlfn.XLOOKUP(B145,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -6942,7 +6939,7 @@
       </c>
       <c r="G145" s="202">
         <f t="shared" si="9"/>
-        <v>1260</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
@@ -7009,7 +7006,7 @@
         <v>565</v>
       </c>
       <c r="E148" s="199">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F148" s="199">
         <f>_xlfn.XLOOKUP(B148,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -7017,7 +7014,7 @@
       </c>
       <c r="G148" s="199">
         <f t="shared" si="9"/>
-        <v>1260</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
@@ -7034,7 +7031,7 @@
         <v>40</v>
       </c>
       <c r="E149" s="199">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="F149" s="199">
         <f>_xlfn.XLOOKUP(B149,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -7042,7 +7039,7 @@
       </c>
       <c r="G149" s="199">
         <f t="shared" si="9"/>
-        <v>642</v>
+        <v>690</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
@@ -7134,7 +7131,7 @@
         <v>565</v>
       </c>
       <c r="E153" s="202">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="F153" s="202">
         <f>_xlfn.XLOOKUP(B153,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -7142,7 +7139,7 @@
       </c>
       <c r="G153" s="202">
         <f t="shared" si="9"/>
-        <v>780</v>
+        <v>900</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -7159,7 +7156,7 @@
         <v>155</v>
       </c>
       <c r="E154" s="199">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="F154" s="199">
         <f>_xlfn.XLOOKUP(B154,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -7167,7 +7164,7 @@
       </c>
       <c r="G154" s="199">
         <f t="shared" si="9"/>
-        <v>270</v>
+        <v>315</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
@@ -7184,7 +7181,7 @@
         <v>155</v>
       </c>
       <c r="E155" s="199">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="F155" s="199">
         <f>_xlfn.XLOOKUP(B155,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -7192,7 +7189,7 @@
       </c>
       <c r="G155" s="199">
         <f t="shared" si="9"/>
-        <v>270</v>
+        <v>363</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
@@ -7305,7 +7302,7 @@
         <v>330</v>
       </c>
       <c r="E160" s="202">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="F160" s="202">
         <v>7</v>
@@ -7314,7 +7311,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" s="202">
         <v>46</v>
       </c>
@@ -7328,7 +7325,7 @@
         <v>330</v>
       </c>
       <c r="E161" s="202">
-        <v>300</v>
+        <v>345</v>
       </c>
       <c r="F161" s="202">
         <v>7</v>
@@ -7337,7 +7334,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" s="199">
         <v>47</v>
       </c>
@@ -7363,7 +7360,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" s="199">
         <v>47</v>
       </c>
@@ -7389,7 +7386,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" s="199">
         <v>47</v>
       </c>
@@ -7404,7 +7401,7 @@
         <v>350</v>
       </c>
       <c r="E164" s="199">
-        <v>200</v>
+        <v>239</v>
       </c>
       <c r="F164" s="199">
         <f>_xlfn.XLOOKUP(B164,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -7412,10 +7409,10 @@
       </c>
       <c r="G164" s="199">
         <f t="shared" si="9"/>
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="199">
         <v>47</v>
       </c>
@@ -7441,7 +7438,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" s="202">
         <v>48</v>
       </c>
@@ -7455,7 +7452,7 @@
         <v>155</v>
       </c>
       <c r="E166" s="202">
-        <v>540</v>
+        <v>560</v>
       </c>
       <c r="F166" s="202">
         <f>_xlfn.XLOOKUP(B166,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -7463,13 +7460,10 @@
       </c>
       <c r="G166" s="202">
         <f t="shared" si="9"/>
-        <v>1620</v>
-      </c>
-      <c r="H166" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" s="202">
         <v>48</v>
       </c>
@@ -7483,7 +7477,7 @@
         <v>155</v>
       </c>
       <c r="E167" s="202">
-        <v>540</v>
+        <v>560</v>
       </c>
       <c r="F167" s="202">
         <f>_xlfn.XLOOKUP(B167,ComponentDuration!$B$2:$B$24,ComponentDuration!$F$2:$F$24)</f>
@@ -7491,10 +7485,10 @@
       </c>
       <c r="G167" s="202">
         <f t="shared" si="9"/>
-        <v>1620</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" s="202">
         <v>48</v>
       </c>
@@ -7519,7 +7513,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" s="202">
         <v>48</v>
       </c>

</xml_diff>